<commit_message>
se mejoran las instrucciones de instalacion para la app y la api | se modifica la carta gantt
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/documentacion/planificacion/Carta Gantt.xlsx
+++ b/Fase 2/Evidencias Proyecto/documentacion/planificacion/Carta Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\duoc\Portafolio\Enmistiempos\Fase 2\Evidencias Proyecto\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\duoc\Portafolio\Enmistiempos\Fase 2\Evidencias Proyecto\documentacion\planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6EF5ED-3662-475D-85A1-E65351041576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BBFF74-3046-4661-9D1F-EE1CDB384097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -709,7 +709,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="5"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">

</xml_diff>